<commit_message>
new input and output file architecture
</commit_message>
<xml_diff>
--- a/file_key.xlsx
+++ b/file_key.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katecrawford/Documents/GitHub/multi_edit_phage/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karen.zhang\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A0033F-5EF7-114A-80AA-12D2AE1E8E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8568B0-DCD4-4F0F-AE02-FC7B517D12C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{5092B66F-C68F-3B49-A10E-6D9E2CEABAC1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{8F0CC697-B677-45A1-A03E-12653B08657D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,138 +36,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
-  <si>
-    <t>phage</t>
-  </si>
-  <si>
-    <t>gene</t>
-  </si>
-  <si>
-    <t>plasmid</t>
-  </si>
-  <si>
-    <t>direction</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>edit_name</t>
   </si>
   <si>
-    <t>genome_position</t>
-  </si>
-  <si>
-    <t>wt_nt</t>
-  </si>
-  <si>
-    <t>edited_nt</t>
-  </si>
-  <si>
-    <t>L_inside</t>
-  </si>
-  <si>
-    <t>R_inside</t>
-  </si>
-  <si>
-    <t>L_outside</t>
-  </si>
-  <si>
-    <t>R_outside</t>
-  </si>
-  <si>
-    <t>rep_1</t>
-  </si>
-  <si>
-    <t>rep_2</t>
-  </si>
-  <si>
-    <t>rep_3</t>
-  </si>
-  <si>
-    <t>rep_4</t>
-  </si>
-  <si>
-    <t>rep_5</t>
-  </si>
-  <si>
-    <t>lambda</t>
-  </si>
-  <si>
-    <t>pSBK164</t>
-  </si>
-  <si>
-    <t>pSBK160</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>CTTTCGCAGT</t>
-  </si>
-  <si>
-    <t>AATCCCATGA</t>
-  </si>
-  <si>
-    <t>TGTAAGTTCCGCAATAACGT</t>
-  </si>
-  <si>
-    <t>CGATGTGCGCCAGCGGAGTC</t>
-  </si>
-  <si>
-    <t>lambda L tail</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>L tail protein</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>CGCAATAACG</t>
-  </si>
-  <si>
-    <t>GTTGTAAGTT</t>
-  </si>
-  <si>
-    <t>TATGACCAGCCAACGTCCGA</t>
-  </si>
-  <si>
-    <t>ACTTTCGCAGTAAATCCCAT</t>
-  </si>
-  <si>
-    <t>L tail dRT</t>
-  </si>
-  <si>
-    <t>msKDC-01-44</t>
-  </si>
-  <si>
-    <t>msKDC-01-45</t>
-  </si>
-  <si>
-    <t>msKDC-01-46</t>
-  </si>
-  <si>
-    <t>msKDC-01-47</t>
-  </si>
-  <si>
-    <t>msKDC-01-48</t>
-  </si>
-  <si>
-    <t>msKDC-01-49</t>
-  </si>
-  <si>
-    <t>msKDC-01-50</t>
+    <t>run_id</t>
+  </si>
+  <si>
+    <t>rpoB</t>
+  </si>
+  <si>
+    <t>msCF_5_35</t>
+  </si>
+  <si>
+    <t>msCF_5_36</t>
+  </si>
+  <si>
+    <t>msCF_5_37</t>
+  </si>
+  <si>
+    <t>msCF_5_38</t>
+  </si>
+  <si>
+    <t>msCF_5_39</t>
+  </si>
+  <si>
+    <t>msCF_5_40</t>
+  </si>
+  <si>
+    <t>msCF_5_41</t>
+  </si>
+  <si>
+    <t>msCF_5_42</t>
+  </si>
+  <si>
+    <t>msCF_5_43</t>
+  </si>
+  <si>
+    <t>msCF_5_44</t>
+  </si>
+  <si>
+    <t>msCF_5_45</t>
+  </si>
+  <si>
+    <t>msCF_5_46</t>
   </si>
 </sst>
 </file>
@@ -173,7 +89,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -186,9 +102,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Helvetica"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -200,12 +116,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -215,7 +146,9 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,200 +462,129 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79934C2-20DB-E449-AFAB-CAA669F7B54D}">
-  <dimension ref="A1:Q23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B6E6236-43F8-4DA8-90EA-4163369B5506}">
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2">
-        <v>14084</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="2">
-        <v>14126</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="P4" s="1"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
had to change pSBK164 left outside search seq because the MiSeq primers sit too close to the donor
</commit_message>
<xml_diff>
--- a/file_key.xlsx
+++ b/file_key.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katecrawford/Documents/GitHub/multi_edit_phage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88682B24-5778-D54F-A8EB-F4BE75E9FEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A43F2AB-E824-294E-B830-E530CF81FA5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36160" yWindow="1480" windowWidth="33600" windowHeight="20500" xr2:uid="{5092B66F-C68F-3B49-A10E-6D9E2CEABAC1}"/>
+    <workbookView xWindow="36160" yWindow="1100" windowWidth="33600" windowHeight="20500" xr2:uid="{5092B66F-C68F-3B49-A10E-6D9E2CEABAC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -137,9 +137,6 @@
     <t>GTTGTAAGTT</t>
   </si>
   <si>
-    <t>TATGACCAGCCAACGTCCGA</t>
-  </si>
-  <si>
     <t>ACTTTCGCAGTAAATCCCAT</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>msAGK-01-79</t>
+  </si>
+  <si>
+    <t>CAACGTCCGATATCACGAAG</t>
   </si>
 </sst>
 </file>
@@ -549,11 +549,12 @@
   <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.6640625" bestFit="1" customWidth="1"/>
@@ -646,25 +647,25 @@
         <v>32</v>
       </c>
       <c r="K2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" t="s">
         <v>34</v>
       </c>
-      <c r="L2" t="s">
-        <v>35</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -681,7 +682,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F3" s="2">
         <v>14126</v>
@@ -705,19 +706,19 @@
         <v>26</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -749,5 +750,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
trying to get Nanopore data to work - it didn't. msCF-9
</commit_message>
<xml_diff>
--- a/file_key.xlsx
+++ b/file_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katecrawford/Documents/GitHub/multi_edit_phage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA2E2E2-271C-364B-8AAE-BF6E43F96804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F65C9E-EA63-0D49-934C-0DEF65A1BF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="700" windowWidth="33600" windowHeight="20500" xr2:uid="{5092B66F-C68F-3B49-A10E-6D9E2CEABAC1}"/>
+    <workbookView xWindow="35420" yWindow="700" windowWidth="33600" windowHeight="20500" xr2:uid="{5092B66F-C68F-3B49-A10E-6D9E2CEABAC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>phage</t>
   </si>
@@ -119,7 +119,10 @@
     <t>CAACGTCCGATATCACGAAG</t>
   </si>
   <si>
-    <t>msMRM-04-155</t>
+    <t>msCF-9-22</t>
+  </si>
+  <si>
+    <t>msCF-9-23</t>
   </si>
 </sst>
 </file>
@@ -601,7 +604,9 @@
       <c r="M2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="3"/>
+      <c r="N2" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>

</xml_diff>

<commit_message>
msCF-9 typo in file key
</commit_message>
<xml_diff>
--- a/file_key.xlsx
+++ b/file_key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katecrawford/Documents/GitHub/multi_edit_phage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8537482E-A7D2-6248-8F71-2F0342C5EFB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB90B2AA-2E6D-A849-A20A-66067CCF2A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34180" yWindow="920" windowWidth="33600" windowHeight="20500" xr2:uid="{5092B66F-C68F-3B49-A10E-6D9E2CEABAC1}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>phage</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>msCF-9-22</t>
+  </si>
+  <si>
+    <t>msCF-9-23</t>
   </si>
 </sst>
 </file>
@@ -495,7 +498,7 @@
   <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,7 +605,7 @@
         <v>28</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>

</xml_diff>

<commit_message>
msPRR_01 correct file key
</commit_message>
<xml_diff>
--- a/file_key.xlsx
+++ b/file_key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katecrawford/Documents/GitHub/multi_edit_phage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD40947B-F6B1-3C44-ABC7-A0482A05DD32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3971A763-1221-C643-8940-75CB620DE895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{5092B66F-C68F-3B49-A10E-6D9E2CEABAC1}"/>
   </bookViews>
@@ -157,121 +157,7 @@
     <t>TCGCGATATTCAACGTCTTA</t>
   </si>
   <si>
-    <t>msPRR-01-02</t>
-  </si>
-  <si>
-    <t>msPRR-01-03</t>
-  </si>
-  <si>
-    <t>msPRR-01-04</t>
-  </si>
-  <si>
-    <t>msPRR-01-05</t>
-  </si>
-  <si>
-    <t>msPRR-01-06</t>
-  </si>
-  <si>
-    <t>msPRR-01-07</t>
-  </si>
-  <si>
-    <t>msPRR-01-08</t>
-  </si>
-  <si>
-    <t>msPRR-01-09</t>
-  </si>
-  <si>
-    <t>msPRR-01-10</t>
-  </si>
-  <si>
-    <t>msPRR-01-11</t>
-  </si>
-  <si>
-    <t>msPRR-01-12</t>
-  </si>
-  <si>
-    <t>msPRR-01-13</t>
-  </si>
-  <si>
-    <t>msPRR-01-14</t>
-  </si>
-  <si>
-    <t>msPRR-01-15</t>
-  </si>
-  <si>
-    <t>msPRR-01-16</t>
-  </si>
-  <si>
-    <t>msPRR-01-17</t>
-  </si>
-  <si>
-    <t>msPRR-01-18</t>
-  </si>
-  <si>
-    <t>msPRR-01-19</t>
-  </si>
-  <si>
-    <t>msPRR-01-20</t>
-  </si>
-  <si>
-    <t>msPRR-01-21</t>
-  </si>
-  <si>
-    <t>msPRR-01-22</t>
-  </si>
-  <si>
-    <t>msPRR-01-23</t>
-  </si>
-  <si>
-    <t>msPRR-01-24</t>
-  </si>
-  <si>
-    <t>msPRR-01-25</t>
-  </si>
-  <si>
-    <t>msPRR-01-26</t>
-  </si>
-  <si>
-    <t>msPRR-01-27</t>
-  </si>
-  <si>
-    <t>msPRR-01-28</t>
-  </si>
-  <si>
-    <t>msPRR-01-29</t>
-  </si>
-  <si>
-    <t>msPRR-01-30</t>
-  </si>
-  <si>
-    <t>msPRR-01-31</t>
-  </si>
-  <si>
-    <t>msPRR-01-32</t>
-  </si>
-  <si>
-    <t>msPRR-01-33</t>
-  </si>
-  <si>
-    <t>msPRR-01-34</t>
-  </si>
-  <si>
-    <t>msPRR-01-35</t>
-  </si>
-  <si>
-    <t>msPRR-01-36</t>
-  </si>
-  <si>
-    <t>msPRR-01-37</t>
-  </si>
-  <si>
-    <t>msPRR-01-38</t>
-  </si>
-  <si>
-    <t>msPRR-01-39</t>
-  </si>
-  <si>
-    <t>msPRR-01-40</t>
+    <t>msPRR_01_02</t>
   </si>
   <si>
     <t>M13</t>
@@ -304,36 +190,6 @@
     <t>TTCGCCCTTTGACGTTGGAG</t>
   </si>
   <si>
-    <t>msPRR-01-41</t>
-  </si>
-  <si>
-    <t>msPRR-01-42</t>
-  </si>
-  <si>
-    <t>msPRR-01-43</t>
-  </si>
-  <si>
-    <t>msPRR-01-44</t>
-  </si>
-  <si>
-    <t>msPRR-01-45</t>
-  </si>
-  <si>
-    <t>msPRR-01-46</t>
-  </si>
-  <si>
-    <t>msPRR-01-47</t>
-  </si>
-  <si>
-    <t>msPRR-01-48</t>
-  </si>
-  <si>
-    <t>msPRR-01-49</t>
-  </si>
-  <si>
-    <t>msPRR-01-50</t>
-  </si>
-  <si>
     <t>pSBK.190</t>
   </si>
   <si>
@@ -349,31 +205,175 @@
     <t>rep4_tc</t>
   </si>
   <si>
-    <t>msPRR-01-51</t>
-  </si>
-  <si>
-    <t>msPRR-01-52</t>
-  </si>
-  <si>
-    <t>msPRR-01-53</t>
-  </si>
-  <si>
-    <t>msPRR-01-186</t>
-  </si>
-  <si>
-    <t>msPRR-01-187</t>
-  </si>
-  <si>
-    <t>msPRR-01-188</t>
-  </si>
-  <si>
-    <t>msPRR-01-189</t>
-  </si>
-  <si>
-    <t>msPRR-01-190</t>
-  </si>
-  <si>
-    <t>msPRR-01-191</t>
+    <t>msPRR_01_04</t>
+  </si>
+  <si>
+    <t>msPRR_01_05</t>
+  </si>
+  <si>
+    <t>msPRR_01_06</t>
+  </si>
+  <si>
+    <t>msPRR_01_07</t>
+  </si>
+  <si>
+    <t>msPRR_01_08</t>
+  </si>
+  <si>
+    <t>msPRR_01_09</t>
+  </si>
+  <si>
+    <t>msPRR_01_10</t>
+  </si>
+  <si>
+    <t>msPRR_01_11</t>
+  </si>
+  <si>
+    <t>msPRR_01_12</t>
+  </si>
+  <si>
+    <t>msPRR_01_13</t>
+  </si>
+  <si>
+    <t>msPRR_01_14</t>
+  </si>
+  <si>
+    <t>msPRR_01_15</t>
+  </si>
+  <si>
+    <t>msPRR_01_16</t>
+  </si>
+  <si>
+    <t>msPRR_01_17</t>
+  </si>
+  <si>
+    <t>msPRR_01_18</t>
+  </si>
+  <si>
+    <t>msPRR_01_19</t>
+  </si>
+  <si>
+    <t>msPRR_01_20</t>
+  </si>
+  <si>
+    <t>msPRR_01_21</t>
+  </si>
+  <si>
+    <t>msPRR_01_22</t>
+  </si>
+  <si>
+    <t>msPRR_01_23</t>
+  </si>
+  <si>
+    <t>msPRR_01_24</t>
+  </si>
+  <si>
+    <t>msPRR_01_25</t>
+  </si>
+  <si>
+    <t>msPRR_01_26</t>
+  </si>
+  <si>
+    <t>msPRR_01_27</t>
+  </si>
+  <si>
+    <t>msPRR_01_28</t>
+  </si>
+  <si>
+    <t>msPRR_01_29</t>
+  </si>
+  <si>
+    <t>msPRR_01_30</t>
+  </si>
+  <si>
+    <t>msPRR_01_31</t>
+  </si>
+  <si>
+    <t>msPRR_01_32</t>
+  </si>
+  <si>
+    <t>msPRR_01_33</t>
+  </si>
+  <si>
+    <t>msPRR_01_34</t>
+  </si>
+  <si>
+    <t>msPRR_01_35</t>
+  </si>
+  <si>
+    <t>msPRR_01_36</t>
+  </si>
+  <si>
+    <t>msPRR_01_37</t>
+  </si>
+  <si>
+    <t>msPRR_01_38</t>
+  </si>
+  <si>
+    <t>msPRR_01_39</t>
+  </si>
+  <si>
+    <t>msPRR_01_40</t>
+  </si>
+  <si>
+    <t>msPRR_01_41</t>
+  </si>
+  <si>
+    <t>msPRR_01_42</t>
+  </si>
+  <si>
+    <t>msPRR_01_43</t>
+  </si>
+  <si>
+    <t>msPRR_01_44</t>
+  </si>
+  <si>
+    <t>msPRR_01_45</t>
+  </si>
+  <si>
+    <t>msPRR_01_46</t>
+  </si>
+  <si>
+    <t>msPRR_01_47</t>
+  </si>
+  <si>
+    <t>msPRR_01_48</t>
+  </si>
+  <si>
+    <t>msPRR_01_49</t>
+  </si>
+  <si>
+    <t>msPRR_01_50</t>
+  </si>
+  <si>
+    <t>msPRR_01_186</t>
+  </si>
+  <si>
+    <t>msPRR_01_187</t>
+  </si>
+  <si>
+    <t>msPRR_01_188</t>
+  </si>
+  <si>
+    <t>msPRR_01_189</t>
+  </si>
+  <si>
+    <t>msPRR_01_190</t>
+  </si>
+  <si>
+    <t>msPRR_01_191</t>
+  </si>
+  <si>
+    <t>msPRR_01_51</t>
+  </si>
+  <si>
+    <t>msPRR_01_52</t>
+  </si>
+  <si>
+    <t>msPRR_01_53</t>
+  </si>
+  <si>
+    <t>msPRR_01_03</t>
   </si>
 </sst>
 </file>
@@ -821,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79934C2-20DB-E449-AFAB-CAA669F7B54D}">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="215" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -930,13 +930,13 @@
         <v>40</v>
       </c>
       <c r="O2" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="P2" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -977,19 +977,19 @@
         <v>39</v>
       </c>
       <c r="M3" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="N3" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="O3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -1030,19 +1030,19 @@
         <v>39</v>
       </c>
       <c r="M4" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="N4" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="O4" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -1083,19 +1083,19 @@
         <v>39</v>
       </c>
       <c r="M5" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="N5" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="O5" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -1136,19 +1136,19 @@
         <v>39</v>
       </c>
       <c r="M6" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="N6" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="O6" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -1189,19 +1189,19 @@
         <v>39</v>
       </c>
       <c r="M7" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="N7" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="O7" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="P7" s="8" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -1242,19 +1242,19 @@
         <v>39</v>
       </c>
       <c r="M8" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="N8" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="O8" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -1295,36 +1295,36 @@
         <v>39</v>
       </c>
       <c r="M9" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="N9" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="O9" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="F10">
         <v>5704</v>
@@ -1336,48 +1336,48 @@
         <v>23</v>
       </c>
       <c r="I10" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="J10" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="K10" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="L10" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="M10" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="N10" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="O10" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
         <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="F11">
         <v>5704</v>
@@ -1389,31 +1389,31 @@
         <v>23</v>
       </c>
       <c r="I11" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="J11" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="K11" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="L11" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="M11" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="N11" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="O11" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
@@ -1424,13 +1424,13 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="F12" s="9">
         <v>11160</v>
@@ -1454,13 +1454,13 @@
         <v>28</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -1471,13 +1471,13 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
       <c r="F13" s="9">
         <v>11160</v>
@@ -1501,13 +1501,13 @@
         <v>28</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="O13" s="8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
@@ -1518,13 +1518,13 @@
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="F14" s="9">
         <v>11160</v>
@@ -1548,13 +1548,13 @@
         <v>28</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
first try msAGK19 human editing
</commit_message>
<xml_diff>
--- a/file_key.xlsx
+++ b/file_key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katecrawford/Documents/GitHub/multi_edit_phage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67660BE0-95FF-544A-9788-3B078A736CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE026F4-58D0-FD4D-B147-B5205EA6CDD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{5092B66F-C68F-3B49-A10E-6D9E2CEABAC1}"/>
   </bookViews>
@@ -609,11 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79934C2-20DB-E449-AFAB-CAA669F7B54D}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:E16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,7 +654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -742,7 +741,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -771,7 +770,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
@@ -800,7 +799,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -829,7 +828,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -916,7 +915,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>29</v>
       </c>
@@ -945,7 +944,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>31</v>
       </c>
@@ -974,7 +973,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>33</v>
       </c>
@@ -1003,7 +1002,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>35</v>
       </c>
@@ -1090,7 +1089,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>41</v>
       </c>
@@ -1119,7 +1118,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>43</v>
       </c>
@@ -1148,7 +1147,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>45</v>
       </c>
@@ -1177,25 +1176,17 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U21" xr:uid="{C79934C2-20DB-E449-AFAB-CAA669F7B54D}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="165"/>
-        <filter val="166"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
error in filekey msAGK19
</commit_message>
<xml_diff>
--- a/file_key.xlsx
+++ b/file_key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katecrawford/Documents/GitHub/multi_edit_phage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE026F4-58D0-FD4D-B147-B5205EA6CDD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC40BD2-C83A-9040-BEAA-9C5CCCA7ACF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{5092B66F-C68F-3B49-A10E-6D9E2CEABAC1}"/>
   </bookViews>
@@ -46,9 +46,6 @@
     <t>wt_nt</t>
   </si>
   <si>
-    <t>edited_nt</t>
-  </si>
-  <si>
     <t>L_inside</t>
   </si>
   <si>
@@ -197,6 +194,9 @@
   </si>
   <si>
     <t>GGACACATGG</t>
+  </si>
+  <si>
+    <t>edit_nt</t>
   </si>
 </sst>
 </file>
@@ -612,7 +612,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -627,10 +627,10 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -639,541 +639,541 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="C2" s="5">
         <v>156</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="H2" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="C3" s="5">
         <v>165</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="H3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="C4" s="5">
         <v>166</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="H4" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="C5" s="5">
         <v>167</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="H5" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="C6" s="5">
         <v>168</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="H6" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="C7" s="5">
         <v>169</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="H7" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="C8" s="5">
         <v>156</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="H8" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="C9" s="5">
         <v>165</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="H9" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="C10" s="5">
         <v>166</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="H10" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="C11" s="5">
         <v>167</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="H11" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="C12" s="5">
         <v>168</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="H12" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="C13" s="5">
         <v>169</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="H13" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="C14" s="5">
         <v>156</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="H14" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="C15" s="5">
         <v>165</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="H15" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="C16" s="5">
         <v>166</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="H16" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="C17" s="5">
         <v>167</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="H17" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="C18" s="5">
         <v>168</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="H18" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="C19" s="5">
         <v>169</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="H19" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>